<commit_message>
updated Readme file, updated comments , updated few methods
</commit_message>
<xml_diff>
--- a/src/main/java/com/economist/qa/testdata/TheEconomistTestData.xlsx
+++ b/src/main/java/com/economist/qa/testdata/TheEconomistTestData.xlsx
@@ -3,38 +3,40 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8C9587C3-13A7-4DFA-AB51-03AE6808EB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheEconomistTest\src\main\java\com\economist\qa\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4CBD3E-52CA-4AEC-9D7F-C35DE5AE26E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19460" windowHeight="11060" xr2:uid="{34FDA050-3785-497E-AD31-185645D48365}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34FDA050-3785-497E-AD31-185645D48365}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Banking and finance</t>
   </si>
   <si>
     <t>SectorName</t>
+  </si>
+  <si>
+    <t>SearchData</t>
+  </si>
+  <si>
+    <t>Director</t>
   </si>
 </sst>
 </file>
@@ -401,30 +403,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3992364A-FA44-4987-BFCB-5439079BBBF8}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>